<commit_message>
Add QueueService for background import process #63
Import: add QueueService, IBackgroundQueue, BackgroundQueue #63

Import: add ProtocolSet.ImportSuccess #63

Import: add DbProgressNotifier #63

Fix empty DB creation, add handy scripts #63

Fix ObjectDisposedException exception, fix issue #49, add errorsCount to progress #63

Rename ProtocolSet.ImportErrors to ImportErrorCount #63
</commit_message>
<xml_diff>
--- a/ElectionStatistics.Tests/Resources/dag_no_uik_nmbr.xlsx
+++ b/ElectionStatistics.Tests/Resources/dag_no_uik_nmbr.xlsx
@@ -370,13 +370,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK10"/>
+  <dimension ref="A1:AK1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1048546" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1048576" activeCellId="0" sqref="A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.59"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -1508,6 +1511,7 @@
         <v>78</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Remove "Required" attribute from LineNumber.Value #27
LDA: skip null valued LineNumbers #27

Add test cases for #27

Rename deploy.sh -> deploy_staging.sh #27
</commit_message>
<xml_diff>
--- a/ElectionStatistics.Tests/Resources/dag_no_uik_nmbr.xlsx
+++ b/ElectionStatistics.Tests/Resources/dag_no_uik_nmbr.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="85">
   <si>
     <t xml:space="preserve">регион</t>
   </si>
@@ -269,6 +269,12 @@
   </si>
   <si>
     <t xml:space="preserve">УИК №141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">УИК №142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Null-values</t>
   </si>
 </sst>
 </file>
@@ -372,13 +378,29 @@
   </sheetPr>
   <dimension ref="A1:AK1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1048546" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1048576" activeCellId="0" sqref="A1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="2.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="3.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="3.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="15" style="0" width="3.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="27" style="0" width="3.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="193.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1509,6 +1531,23 @@
       </c>
       <c r="AK10" s="0" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK11" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>